<commit_message>
Updated Gcode list M130 command comments
</commit_message>
<xml_diff>
--- a/GCODES_MELT.xlsx
+++ b/GCODES_MELT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="312">
   <si>
     <t xml:space="preserve">Bootloader / Firmware</t>
   </si>
@@ -269,463 +269,470 @@
     <t xml:space="preserve">M130</t>
   </si>
   <si>
+    <t xml:space="preserve">T&lt;kp&gt; U&lt;Ki&gt; V&lt;kd&gt; S&lt;1/0&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define PID vars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1 for bed
+S0 for extruder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print Current PID output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set bed temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set chamber temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define bed setpoint and block movements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?X&lt;VAL&gt; ?Y&lt;VAL&gt; ?Z&lt;VAL&gt; ?E&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define steps por mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?X&lt;VAL&gt; ?Y ?Z ?F ?E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define Acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?X&lt;VAL&gt; ?Y ?Z ?F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set home offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?S&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set speed factor override percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?S&lt;VAL&gt; ?W&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set extrude factor override percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If 1=100%, use W&lt;Val&gt;; if 100=100% use S&lt;Val&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?S&lt;VAL&gt; ?P&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set safe temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clears config shutdown flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M506</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reload Config Vars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print Config Vars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write Current Config Vars to Memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets Home Z Pos to the current Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset Config to Default Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reboots Electronics into Bootloader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print Current Printer Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3: ready</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4: moving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5: printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7: pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9: shutdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alive command, DOES NOT GIVE A RESPONSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M639</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In marlin, this command echoes a string to the LCD. The M70 command as a similar function. Since this command is already being used in bootloader and firmware to report the printer serial number it stays unchanged.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pause sd printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A&lt;0/1&gt; ?S&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter/Exit Power saving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?S&lt;FeedRate_Coef&gt; ?T&lt;Temperature&gt;, ?W&lt;FlowRate&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resume sd printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficients: 1.0 = 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Filament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unload Filament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Heating Procedure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel Heating Procedure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Filament String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Filament String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Last Print Time (milliseconds)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S&lt;VAL MM&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Filament in Spool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Filament in Spool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send last print filament consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S&lt;VAL MICRONS&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Nozzle Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Nozzle Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send Extruder log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?S&lt;0/1&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Debug Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define seconds to enter in power saving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pause at Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print door state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open/Close Door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set encoder position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?X&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set encoder steps/mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?L&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set encoder Max error before failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print Extrusion Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?S&lt;1/0&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable/Disable encode failure print pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get current line number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable/Disable Door protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A&lt;VAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Firmware Version String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print Bootloader Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print Serial Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write Serial Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTF+,BE ME, BE School, BTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to Firmware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets printer to receive A bytes to firmware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M651</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prints Firmware State Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Firmware and Config Memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets printer to receive A bytes to firmware and clears config memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open file to write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defione variables of standalone print</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print variables of standalone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print selected file to USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turn Extruder fan ON, or define Extruder fan speed (0-255)</t>
+  </si>
+  <si>
     <t xml:space="preserve">T&lt;kp&gt; U&lt;Ki&gt; V&lt;kd&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Define PID vars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print Current PID output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set bed temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set chamber temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Define bed setpoint and block movements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?X&lt;VAL&gt; ?Y&lt;VAL&gt; ?Z&lt;VAL&gt; ?E&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Define steps por mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?X&lt;VAL&gt; ?Y ?Z ?F ?E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Define Acceleration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?X&lt;VAL&gt; ?Y ?Z ?F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set home offset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?S&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set speed factor override percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?S&lt;VAL&gt; ?W&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set extrude factor override percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If 1=100%, use W&lt;Val&gt;; if 100=100% use S&lt;Val&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?S&lt;VAL&gt; ?P&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set safe temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clears config shutdown flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M506</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reload Config Vars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print Config Vars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M601</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Write Current Config Vars to Memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sets Home Z Pos to the current Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M607</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reset Config to Default Values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M609</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reboots Electronics into Bootloader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print Current Printer Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3: ready</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4: moving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5: printing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7: pause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9: shutdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M637</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alive command, DOES NOT GIVE A RESPONSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M639</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">echo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In marlin, this command echoes a string to the LCD. The M70 command as a similar function. Since this command is already being used in bootloader and firmware to report the printer serial number it stays unchanged.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M640</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pause sd printing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M641</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A&lt;0/1&gt; ?S&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter/Exit Power saving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M642</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M643</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?S&lt;FeedRate_Coef&gt; ?T&lt;Temperature&gt;, ?W&lt;FlowRate&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resume sd printing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficients: 1.0 = 100%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load Filament</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M702</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unload Filament</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Heating Procedure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M704</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancel Heating Procedure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set Filament String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read Filament String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report Last Print Time (milliseconds)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S&lt;VAL MM&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set Filament in Spool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get Filament in Spool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Send last print filament consumption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S&lt;VAL MICRONS&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set Nozzle Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report Nozzle Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Send Extruder log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?S&lt;0/1&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set Debug Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Define seconds to enter in power saving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pause at Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print door state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open/Close Door</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set encoder position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?X&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set encoder steps/mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?L&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set encoder Max error before failure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print Extrusion Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?S&lt;1/0&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable/Disable encode failure print pause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1305</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get current line number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M1306</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable/Disable Door protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A&lt;VAL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set Firmware Version String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print Bootloader Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M117</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print Serial Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Write Serial Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BTF+,BE ME, BE School, BTF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to Firmware</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sets printer to receive A bytes to firmware</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M651</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prints Firmware State Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M652</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read Firmware and Config Memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M653</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sets printer to receive A bytes to firmware and clears config memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open file to write</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defione variables of standalone print</t>
-  </si>
-  <si>
-    <t xml:space="preserve">print variables of standalone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print selected file to USB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turn Extruder fan ON, or define Extruder fan speed (0-255)</t>
   </si>
   <si>
     <t xml:space="preserve">Define Home position</t>
@@ -1637,8 +1644,8 @@
   </sheetPr>
   <dimension ref="1:75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1967,7 +1974,9 @@
       <c r="D20" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="F20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1975,13 +1984,13 @@
         <v>7</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="16"/>
@@ -1991,13 +2000,13 @@
         <v>7</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="16"/>
@@ -2007,13 +2016,13 @@
         <v>7</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="16"/>
@@ -2023,13 +2032,13 @@
         <v>7</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="16"/>
@@ -2039,13 +2048,13 @@
         <v>7</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="16"/>
@@ -2055,13 +2064,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="16"/>
@@ -2071,13 +2080,13 @@
         <v>7</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="16"/>
@@ -2087,13 +2096,13 @@
         <v>7</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="16"/>
@@ -2103,16 +2112,16 @@
         <v>7</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F29" s="16"/>
     </row>
@@ -2121,13 +2130,13 @@
         <v>7</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="16"/>
@@ -2137,13 +2146,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="16"/>
@@ -2153,13 +2162,13 @@
         <v>7</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E32" s="18"/>
     </row>
@@ -2168,13 +2177,13 @@
         <v>7</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="16"/>
@@ -2184,13 +2193,13 @@
         <v>7</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E34" s="18"/>
       <c r="F34" s="16"/>
@@ -2200,13 +2209,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="16"/>
@@ -2216,13 +2225,13 @@
         <v>7</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="16"/>
@@ -2232,13 +2241,13 @@
         <v>7</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="16"/>
@@ -2248,13 +2257,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E38" s="19"/>
     </row>
@@ -2263,13 +2272,13 @@
         <v>7</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="20"/>
@@ -2279,7 +2288,7 @@
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E40" s="19"/>
       <c r="F40" s="20"/>
@@ -2289,7 +2298,7 @@
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E41" s="19"/>
       <c r="F41" s="20"/>
@@ -2299,7 +2308,7 @@
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="20"/>
@@ -2309,7 +2318,7 @@
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="20"/>
@@ -2319,7 +2328,7 @@
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E44" s="19"/>
       <c r="F44" s="20"/>
@@ -2329,13 +2338,13 @@
         <v>7</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E45" s="19"/>
     </row>
@@ -2344,16 +2353,16 @@
         <v>7</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F46" s="16"/>
     </row>
@@ -2362,13 +2371,13 @@
         <v>7</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E47" s="18"/>
     </row>
@@ -2377,13 +2386,13 @@
         <v>7</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E48" s="19"/>
     </row>
@@ -2392,16 +2401,16 @@
         <v>7</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F49" s="16"/>
     </row>
@@ -2410,16 +2419,16 @@
         <v>7</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2427,13 +2436,13 @@
         <v>7</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E51" s="19"/>
     </row>
@@ -2442,13 +2451,13 @@
         <v>7</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E52" s="19"/>
     </row>
@@ -2457,13 +2466,13 @@
         <v>7</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E53" s="19"/>
     </row>
@@ -2472,13 +2481,13 @@
         <v>7</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E54" s="19"/>
     </row>
@@ -2487,13 +2496,13 @@
         <v>7</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>40</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E55" s="18"/>
     </row>
@@ -2502,13 +2511,13 @@
         <v>7</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C56" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E56" s="18"/>
     </row>
@@ -2517,13 +2526,13 @@
         <v>7</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E57" s="18"/>
     </row>
@@ -2532,13 +2541,13 @@
         <v>7</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E58" s="19"/>
     </row>
@@ -2547,13 +2556,13 @@
         <v>7</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C59" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E59" s="19"/>
     </row>
@@ -2562,13 +2571,13 @@
         <v>7</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E60" s="19"/>
     </row>
@@ -2577,13 +2586,13 @@
         <v>7</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E61" s="19"/>
     </row>
@@ -2592,13 +2601,13 @@
         <v>7</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E62" s="19"/>
     </row>
@@ -2607,13 +2616,13 @@
         <v>7</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E63" s="19"/>
     </row>
@@ -2622,13 +2631,13 @@
         <v>7</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E64" s="19"/>
     </row>
@@ -2637,13 +2646,13 @@
         <v>7</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E65" s="19"/>
     </row>
@@ -2652,13 +2661,13 @@
         <v>7</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E66" s="18"/>
     </row>
@@ -2667,13 +2676,13 @@
         <v>7</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E67" s="18"/>
     </row>
@@ -2682,13 +2691,13 @@
         <v>7</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E68" s="18"/>
     </row>
@@ -2697,13 +2706,13 @@
         <v>7</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E69" s="19"/>
     </row>
@@ -2711,10 +2720,10 @@
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E70" s="19"/>
     </row>
@@ -2722,10 +2731,10 @@
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E71" s="19"/>
     </row>
@@ -2734,13 +2743,13 @@
         <v>7</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C72" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E72" s="19"/>
     </row>
@@ -2749,13 +2758,13 @@
         <v>7</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E73" s="19"/>
     </row>
@@ -2764,13 +2773,13 @@
         <v>7</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C74" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D74" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E74" s="19"/>
     </row>
@@ -2779,13 +2788,13 @@
         <v>7</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E75" s="19"/>
     </row>
@@ -2855,22 +2864,22 @@
     </row>
     <row r="2" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2895,13 +2904,13 @@
     </row>
     <row r="4" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
@@ -2910,7 +2919,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2918,10 +2927,10 @@
         <v>76</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
@@ -2930,127 +2939,127 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3149,13 +3158,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3205,13 +3214,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3225,7 +3234,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3239,7 +3248,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3261,13 +3270,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3387,13 +3396,13 @@
         <v>76</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C22" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3415,13 +3424,13 @@
         <v>7</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3432,7 +3441,7 @@
         <v>79</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>80</v>
+        <v>234</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>81</v>
@@ -3443,37 +3452,37 @@
         <v>7</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="24"/>
       <c r="B27" s="25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="24"/>
       <c r="B28" s="25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3481,13 +3490,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3503,13 +3512,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3517,13 +3526,13 @@
         <v>7</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3531,13 +3540,13 @@
         <v>7</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3545,13 +3554,13 @@
         <v>7</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3559,13 +3568,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3573,13 +3582,13 @@
         <v>7</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3587,13 +3596,13 @@
         <v>7</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3601,13 +3610,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C38" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3615,13 +3624,13 @@
         <v>7</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3629,13 +3638,13 @@
         <v>7</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3643,13 +3652,13 @@
         <v>7</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3657,13 +3666,13 @@
         <v>7</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3671,13 +3680,13 @@
         <v>7</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3685,13 +3694,13 @@
         <v>76</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C44" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3699,13 +3708,13 @@
         <v>7</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3713,7 +3722,7 @@
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>
       <c r="D46" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3721,7 +3730,7 @@
       <c r="B47" s="26"/>
       <c r="C47" s="26"/>
       <c r="D47" s="24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3729,7 +3738,7 @@
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
       <c r="D48" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3737,7 +3746,7 @@
       <c r="B49" s="26"/>
       <c r="C49" s="26"/>
       <c r="D49" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3745,21 +3754,21 @@
       <c r="B50" s="26"/>
       <c r="C50" s="26"/>
       <c r="D50" s="24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="24" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3767,13 +3776,13 @@
         <v>7</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C52" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3781,13 +3790,13 @@
         <v>7</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3795,13 +3804,13 @@
         <v>7</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C54" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3809,13 +3818,13 @@
         <v>7</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C55" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3823,13 +3832,13 @@
         <v>7</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3837,13 +3846,13 @@
         <v>7</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3851,13 +3860,13 @@
         <v>7</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3865,13 +3874,13 @@
         <v>7</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3879,13 +3888,13 @@
         <v>7</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C60" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3893,13 +3902,13 @@
         <v>7</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C61" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3907,13 +3916,13 @@
         <v>7</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C62" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3921,13 +3930,13 @@
         <v>7</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C63" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3935,13 +3944,13 @@
         <v>7</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C64" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3949,13 +3958,13 @@
         <v>7</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C65" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3963,13 +3972,13 @@
         <v>7</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C66" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3977,13 +3986,13 @@
         <v>7</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C67" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D67" s="24" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3991,93 +4000,93 @@
         <v>7</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C68" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="24"/>
       <c r="B69" s="25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="24"/>
       <c r="B70" s="25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C70" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="24"/>
       <c r="B71" s="25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="24"/>
       <c r="B72" s="26" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C72" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="24"/>
       <c r="B73" s="26"/>
       <c r="C73" s="24" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D73" s="24" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="24"/>
       <c r="B74" s="26"/>
       <c r="C74" s="24" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="24"/>
       <c r="B75" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C75" s="29" t="s">
         <v>15</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4085,13 +4094,13 @@
         <v>7</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D76" s="29" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4162,16 +4171,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4179,16 +4188,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>262</v>
-      </c>
       <c r="E3" s="24" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4247,7 +4256,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>15</v>
@@ -4256,7 +4265,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4315,7 +4324,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>40</v>
@@ -4324,7 +4333,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4341,7 +4350,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4358,7 +4367,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4383,7 +4392,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>15</v>
@@ -4392,7 +4401,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4536,7 +4545,7 @@
         <v>76</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>15</v>
@@ -4545,7 +4554,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4570,7 +4579,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>62</v>
@@ -4579,7 +4588,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4587,16 +4596,16 @@
         <v>7</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4604,16 +4613,16 @@
         <v>7</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4621,16 +4630,16 @@
         <v>7</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4639,7 +4648,7 @@
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" s="24" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4647,23 +4656,23 @@
         <v>7</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="24" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
@@ -4672,7 +4681,7 @@
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="24" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="26"/>
@@ -4681,7 +4690,7 @@
       <c r="A34" s="26"/>
       <c r="B34" s="26"/>
       <c r="C34" s="24" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
@@ -4694,7 +4703,7 @@
         <v>79</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>80</v>
+        <v>234</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>10</v>
@@ -4708,7 +4717,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>15</v>
@@ -4717,7 +4726,7 @@
         <v>10</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4725,16 +4734,16 @@
         <v>7</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4742,16 +4751,16 @@
         <v>7</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C38" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4759,16 +4768,16 @@
         <v>7</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4776,16 +4785,16 @@
         <v>7</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4793,7 +4802,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>9</v>
@@ -4802,7 +4811,7 @@
         <v>10</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4819,16 +4828,16 @@
         <v>7</v>
       </c>
       <c r="B43" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="24" t="s">
         <v>96</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4836,16 +4845,16 @@
         <v>7</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D44" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4853,16 +4862,16 @@
         <v>7</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D45" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4870,16 +4879,16 @@
         <v>7</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D46" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4887,16 +4896,16 @@
         <v>7</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4904,7 +4913,7 @@
         <v>7</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>15</v>
@@ -4913,7 +4922,7 @@
         <v>10</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4921,7 +4930,7 @@
         <v>7</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>15</v>
@@ -4930,7 +4939,7 @@
         <v>10</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4938,7 +4947,7 @@
         <v>7</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C50" s="24" t="s">
         <v>15</v>
@@ -4947,7 +4956,7 @@
         <v>10</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4955,7 +4964,7 @@
         <v>7</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>15</v>
@@ -4964,7 +4973,7 @@
         <v>10</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4972,7 +4981,7 @@
         <v>7</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C52" s="24" t="s">
         <v>15</v>
@@ -4981,7 +4990,7 @@
         <v>10</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4989,7 +4998,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>9</v>
@@ -4998,7 +5007,7 @@
         <v>10</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5006,7 +5015,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C54" s="24" t="s">
         <v>9</v>
@@ -5015,7 +5024,7 @@
         <v>10</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5023,7 +5032,7 @@
         <v>7</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C55" s="24" t="s">
         <v>15</v>
@@ -5032,7 +5041,7 @@
         <v>10</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5040,7 +5049,7 @@
         <v>76</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>15</v>
@@ -5049,7 +5058,7 @@
         <v>10</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5057,7 +5066,7 @@
         <v>7</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C57" s="26" t="s">
         <v>15</v>
@@ -5066,7 +5075,7 @@
         <v>10</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5075,7 +5084,7 @@
       <c r="C58" s="26"/>
       <c r="D58" s="26"/>
       <c r="E58" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5084,7 +5093,7 @@
       <c r="C59" s="26"/>
       <c r="D59" s="26"/>
       <c r="E59" s="24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5093,7 +5102,7 @@
       <c r="C60" s="26"/>
       <c r="D60" s="26"/>
       <c r="E60" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5102,7 +5111,7 @@
       <c r="C61" s="26"/>
       <c r="D61" s="26"/>
       <c r="E61" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5111,15 +5120,15 @@
       <c r="C62" s="26"/>
       <c r="D62" s="26"/>
       <c r="E62" s="24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="24" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C63" s="24" t="s">
         <v>15</v>
@@ -5128,7 +5137,7 @@
         <v>10</v>
       </c>
       <c r="E63" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5136,7 +5145,7 @@
         <v>7</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C64" s="24" t="s">
         <v>15</v>
@@ -5145,7 +5154,7 @@
         <v>10</v>
       </c>
       <c r="E64" s="24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5153,7 +5162,7 @@
         <v>7</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C65" s="24" t="s">
         <v>15</v>
@@ -5162,7 +5171,7 @@
         <v>10</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5170,7 +5179,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C66" s="24" t="s">
         <v>15</v>
@@ -5179,7 +5188,7 @@
         <v>10</v>
       </c>
       <c r="E66" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5187,7 +5196,7 @@
         <v>7</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C67" s="24" t="s">
         <v>15</v>
@@ -5196,7 +5205,7 @@
         <v>10</v>
       </c>
       <c r="E67" s="24" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5204,16 +5213,16 @@
         <v>7</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D68" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E68" s="24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5221,16 +5230,16 @@
         <v>7</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D69" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E69" s="24" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5238,16 +5247,16 @@
         <v>7</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D70" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E70" s="24" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5255,7 +5264,7 @@
         <v>7</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C71" s="24" t="s">
         <v>15</v>
@@ -5264,7 +5273,7 @@
         <v>10</v>
       </c>
       <c r="E71" s="24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5272,7 +5281,7 @@
         <v>7</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C72" s="24" t="s">
         <v>15</v>
@@ -5281,7 +5290,7 @@
         <v>10</v>
       </c>
       <c r="E72" s="24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5289,7 +5298,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C73" s="24" t="s">
         <v>62</v>
@@ -5298,7 +5307,7 @@
         <v>10</v>
       </c>
       <c r="E73" s="24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5306,7 +5315,7 @@
         <v>7</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C74" s="24" t="s">
         <v>15</v>
@@ -5315,7 +5324,7 @@
         <v>10</v>
       </c>
       <c r="E74" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5323,7 +5332,7 @@
         <v>7</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C75" s="24" t="s">
         <v>40</v>
@@ -5332,7 +5341,7 @@
         <v>10</v>
       </c>
       <c r="E75" s="24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5340,7 +5349,7 @@
         <v>7</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>15</v>
@@ -5349,7 +5358,7 @@
         <v>10</v>
       </c>
       <c r="E76" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5357,7 +5366,7 @@
         <v>7</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C77" s="24" t="s">
         <v>15</v>
@@ -5366,7 +5375,7 @@
         <v>10</v>
       </c>
       <c r="E77" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5374,7 +5383,7 @@
         <v>7</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>15</v>
@@ -5383,7 +5392,7 @@
         <v>10</v>
       </c>
       <c r="E78" s="24" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5391,16 +5400,16 @@
         <v>7</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D79" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5408,7 +5417,7 @@
         <v>7</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C80" s="24" t="s">
         <v>15</v>
@@ -5417,7 +5426,7 @@
         <v>10</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5425,16 +5434,16 @@
         <v>7</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D81" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E81" s="24" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5442,16 +5451,16 @@
         <v>7</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D82" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E82" s="24" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5459,16 +5468,16 @@
         <v>7</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C83" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D83" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E83" s="24" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5476,16 +5485,16 @@
         <v>7</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C84" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D84" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E84" s="24" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5493,16 +5502,16 @@
         <v>7</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C85" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D85" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E85" s="24" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5510,16 +5519,16 @@
         <v>7</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C86" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D86" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E86" s="24" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5527,16 +5536,16 @@
         <v>7</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C87" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D87" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E87" s="24" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5544,16 +5553,16 @@
         <v>7</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D88" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E88" s="24" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5561,16 +5570,16 @@
         <v>7</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C89" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D89" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E89" s="24" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5578,16 +5587,16 @@
         <v>7</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C90" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D90" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E90" s="24" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5595,7 +5604,7 @@
         <v>7</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C91" s="24" t="s">
         <v>62</v>
@@ -5604,7 +5613,7 @@
         <v>10</v>
       </c>
       <c r="E91" s="24" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5612,7 +5621,7 @@
         <v>7</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C92" s="24" t="s">
         <v>62</v>
@@ -5621,7 +5630,7 @@
         <v>10</v>
       </c>
       <c r="E92" s="24" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5629,16 +5638,16 @@
         <v>7</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C93" s="29" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D93" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E93" s="29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added entry to Gcode list
</commit_message>
<xml_diff>
--- a/GCODES_MELT.xlsx
+++ b/GCODES_MELT.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="313">
   <si>
     <t>Bootloader / Firmware</t>
   </si>
@@ -797,9 +797,6 @@
   </si>
   <si>
     <t>S&lt;BOOL&gt;</t>
-  </si>
-  <si>
-    <t>Activate/deactivate door latch</t>
   </si>
   <si>
     <t>Set Encoder position</t>
@@ -1210,16 +1207,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1586,64 +1583,64 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="27" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="30" t="s">
+      <c r="A4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="27" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -1746,34 +1743,34 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="27" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
@@ -1817,21 +1814,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1.3937007874015748" bottom="1.3937007874015748" header="1" footer="1"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4276,8 +4273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMF1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="43.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6243,15 +6240,9 @@
     </row>
     <row r="71" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="23"/>
-      <c r="B71" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>254</v>
-      </c>
-      <c r="D71" s="23" t="s">
-        <v>255</v>
-      </c>
+      <c r="B71" s="24"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
     </row>
     <row r="72" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="23"/>
@@ -6262,27 +6253,27 @@
         <v>62</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="23"/>
       <c r="B73" s="33"/>
       <c r="C73" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="D73" s="23" t="s">
         <v>257</v>
-      </c>
-      <c r="D73" s="23" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="23"/>
       <c r="B74" s="33"/>
       <c r="C74" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D74" s="23" t="s">
         <v>259</v>
-      </c>
-      <c r="D74" s="23" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6294,7 +6285,7 @@
         <v>15</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6308,18 +6299,18 @@
         <v>254</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C79" s="23" t="s">
         <v>254</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="1048551" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7418,16 +7409,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>264</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:1021" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7435,16 +7426,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>266</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:1021" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7849,10 +7840,10 @@
         <v>62</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7860,16 +7851,16 @@
         <v>7</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E28" s="23" t="s">
         <v>269</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7877,16 +7868,16 @@
         <v>7</v>
       </c>
       <c r="B29" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="C29" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="D29" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="E29" s="23" t="s">
         <v>272</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7895,7 +7886,7 @@
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7903,23 +7894,23 @@
         <v>7</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C31" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="E31" s="33" t="s">
         <v>275</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
       <c r="C32" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
@@ -7928,7 +7919,7 @@
       <c r="A33" s="33"/>
       <c r="B33" s="33"/>
       <c r="C33" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
@@ -7937,7 +7928,7 @@
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="C34" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
@@ -7981,16 +7972,16 @@
         <v>7</v>
       </c>
       <c r="B37" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E37" s="23" t="s">
         <v>280</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E37" s="23" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7998,16 +7989,16 @@
         <v>7</v>
       </c>
       <c r="B38" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E38" s="23" t="s">
         <v>282</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8015,16 +8006,16 @@
         <v>7</v>
       </c>
       <c r="B39" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="D39" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E39" s="23" t="s">
         <v>285</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8032,16 +8023,16 @@
         <v>7</v>
       </c>
       <c r="B40" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E40" s="23" t="s">
         <v>287</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8143,16 +8134,16 @@
         <v>7</v>
       </c>
       <c r="B47" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E47" s="23" t="s">
         <v>289</v>
-      </c>
-      <c r="C47" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8673,7 +8664,7 @@
         <v>10</v>
       </c>
       <c r="E80" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8681,16 +8672,16 @@
         <v>7</v>
       </c>
       <c r="B81" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C81" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E81" s="23" t="s">
         <v>292</v>
-      </c>
-      <c r="C81" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E81" s="23" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8698,16 +8689,16 @@
         <v>7</v>
       </c>
       <c r="B82" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="C82" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="C82" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D82" s="23" t="s">
+      <c r="E82" s="23" t="s">
         <v>295</v>
-      </c>
-      <c r="E82" s="23" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8721,10 +8712,10 @@
         <v>15</v>
       </c>
       <c r="D83" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E83" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8732,16 +8723,16 @@
         <v>7</v>
       </c>
       <c r="B84" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="C84" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="E84" s="23" t="s">
         <v>298</v>
-      </c>
-      <c r="C84" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D84" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="E84" s="23" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8749,16 +8740,16 @@
         <v>7</v>
       </c>
       <c r="B85" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C85" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="E85" s="23" t="s">
         <v>300</v>
-      </c>
-      <c r="C85" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D85" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="E85" s="23" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8766,16 +8757,16 @@
         <v>7</v>
       </c>
       <c r="B86" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="E86" s="23" t="s">
         <v>302</v>
-      </c>
-      <c r="C86" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D86" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="E86" s="23" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8783,16 +8774,16 @@
         <v>7</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C87" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D87" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E87" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8800,16 +8791,16 @@
         <v>7</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C88" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D88" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E88" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8817,16 +8808,16 @@
         <v>7</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C89" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D89" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E89" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8834,16 +8825,16 @@
         <v>7</v>
       </c>
       <c r="B90" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="C90" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E90" s="23" t="s">
         <v>310</v>
-      </c>
-      <c r="C90" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="E90" s="23" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8908,6 +8899,11 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="B57:B62"/>
     <mergeCell ref="C57:C62"/>
@@ -8919,11 +8915,6 @@
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="D31:D34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1.3937007874015748" bottom="1.3937007874015748" header="1" footer="1"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>